<commit_message>
Generated output for the valueSet change for -  "observation-path-atomic-1" and  "observation-imag-atomic-1" profiles
from

https://healthterminologies.gov.au/fhir/ValueSet/diagnostic-observation-status-1

to:

https://healthterminologies.gov.au/fhir/ValueSet/observationstatus-result-available-1
</commit_message>
<xml_diff>
--- a/output/DiagnosticReport/observation-imag-atomic-1.xlsx
+++ b/output/DiagnosticReport/observation-imag-atomic-1.xlsx
@@ -664,7 +664,7 @@
     <t>required</t>
   </si>
   <si>
-    <t>https://healthterminologies.gov.au/fhir/ValueSet/diagnostic-observation-status-1</t>
+    <t>https://healthterminologies.gov.au/fhir/ValueSet/observationstatus-result-available-1</t>
   </si>
   <si>
     <t>Event.status</t>
@@ -1672,7 +1672,7 @@
     <col min="22" max="22" width="17.078125" customWidth="true" bestFit="true"/>
     <col min="23" max="23" width="16.30859375" customWidth="true" bestFit="true"/>
     <col min="24" max="24" width="60.515625" customWidth="true" bestFit="true"/>
-    <col min="25" max="25" width="74.34765625" customWidth="true" bestFit="true"/>
+    <col min="25" max="25" width="78.2890625" customWidth="true" bestFit="true"/>
     <col min="26" max="26" width="5.69140625" customWidth="true" bestFit="true"/>
     <col min="27" max="27" width="19.73046875" customWidth="true" bestFit="true"/>
     <col min="28" max="28" width="40.03515625" customWidth="true" bestFit="true"/>

</xml_diff>